<commit_message>
thêm xóa sửa lý do kỉ luật
</commit_message>
<xml_diff>
--- a/public/upload/file_mau/danh_sach_ki_luat.xlsx
+++ b/public/upload/file_mau/danh_sach_ki_luat.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="noi_dung_tieu_chi" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>TRƯỜNG ĐẠI HỌC CÔNG NGHỆ SÀI GÒN</t>
   </si>
@@ -62,54 +61,6 @@
   </si>
   <si>
     <t>Tiêu chí trừ điểm</t>
-  </si>
-  <si>
-    <t>ib</t>
-  </si>
-  <si>
-    <t>ia</t>
-  </si>
-  <si>
-    <t>Mã tiêu chí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nội dung </t>
-  </si>
-  <si>
-    <t>a.Ý thức học tập</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b.Kết quả học tập </t>
-  </si>
-  <si>
-    <t>c.Nghiên cứu khoa học, tham gia các hoạt động học thuật</t>
-  </si>
-  <si>
-    <t>II. Ý thức chấp hành nội quy, quy chế, quy định trong nhà trường (0 – 25 điểm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">III. Ý thức tham gia các hoạt động chính trị - xã hội, văn hóa, văn nghệ, thể thao, phòng chống các tệ nạn xã hội (0 – 20 điểm) </t>
-  </si>
-  <si>
-    <t>IV. Ý thức công dân trong quan hệ cộng đồng (0 – 25 điểm)</t>
-  </si>
-  <si>
-    <t>V. Ý thức và kết quả tham gia công tác cán bộ lớp, các đoàn thể, tổ chức khác trong nhà trường hoặc sinh viên đạt được thành tích đặc biệt trong học tập, rèn luyện (0 – 10 điểm)</t>
-  </si>
-  <si>
-    <t>ic</t>
-  </si>
-  <si>
-    <t>ii</t>
-  </si>
-  <si>
-    <t>iii</t>
-  </si>
-  <si>
-    <t>iv</t>
-  </si>
-  <si>
-    <t>v</t>
   </si>
 </sst>
 </file>
@@ -415,6 +366,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -423,18 +386,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,37 +686,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -810,9 +761,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="26"/>
-      <c r="I5" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
@@ -823,9 +772,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="26"/>
-      <c r="I6" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
@@ -836,9 +783,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="26"/>
-      <c r="I7" s="10" t="s">
-        <v>24</v>
-      </c>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
@@ -937,23 +882,23 @@
       <c r="H16" s="25"/>
     </row>
     <row r="17" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="20"/>
-      <c r="D17" s="33"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="21"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
       <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="20"/>
-      <c r="D18" s="33"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="22"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -967,23 +912,23 @@
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
-      <c r="B20" s="32"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="20"/>
-      <c r="D20" s="33"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="21"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="34"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="31"/>
       <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="20"/>
-      <c r="D21" s="33"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="21"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="34"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="31"/>
       <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1008,11 +953,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:I3"/>
@@ -1021,6 +961,11 @@
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1028,7 +973,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>noi_dung_tieu_chi!$A$2:$A$8</xm:f>
+            <xm:f>#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
@@ -1036,87 +981,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="68.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
sửa hiển thị class theo danh sách ính viên chấm của học kì sửa export ajax
</commit_message>
<xml_diff>
--- a/public/upload/file_mau/danh_sach_ki_luat.xlsx
+++ b/public/upload/file_mau/danh_sach_ki_luat.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="noi_dung_tieu_chi" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>TRƯỜNG ĐẠI HỌC CÔNG NGHỆ SÀI GÒN</t>
   </si>
@@ -61,6 +62,27 @@
   </si>
   <si>
     <t>Tiêu chí trừ điểm</t>
+  </si>
+  <si>
+    <t>Mã tiêu chí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nội dung </t>
+  </si>
+  <si>
+    <t>II. Ý thức chấp hành nội quy, quy chế, quy định trong nhà trường (0 – 25 điểm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">III. Ý thức tham gia các hoạt động chính trị - xã hội, văn hóa, văn nghệ, thể thao, phòng chống các tệ nạn xã hội (0 – 20 điểm) </t>
+  </si>
+  <si>
+    <t>IV. Ý thức công dân trong quan hệ cộng đồng (0 – 25 điểm)</t>
+  </si>
+  <si>
+    <t>V. Ý thức và kết quả tham gia công tác cán bộ lớp, các đoàn thể, tổ chức khác trong nhà trường hoặc sinh viên đạt được thành tích đặc biệt trong học tập, rèn luyện (0 – 10 điểm)</t>
+  </si>
+  <si>
+    <t>I. Ý thức tham gia học tập (0 – 20 điểm)</t>
   </si>
 </sst>
 </file>
@@ -366,6 +388,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -377,15 +408,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -670,7 +692,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,37 +708,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -882,23 +904,23 @@
       <c r="H16" s="25"/>
     </row>
     <row r="17" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="20"/>
-      <c r="D17" s="30"/>
+      <c r="D17" s="33"/>
       <c r="E17" s="21"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
       <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="20"/>
-      <c r="D18" s="30"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="22"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -912,23 +934,23 @@
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="20"/>
-      <c r="D20" s="30"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="21"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="34"/>
       <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="29"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="32"/>
       <c r="C21" s="20"/>
-      <c r="D21" s="30"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="21"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -953,6 +975,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:I3"/>
@@ -961,11 +988,6 @@
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -973,7 +995,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>#REF!</xm:f>
+            <xm:f>noi_dung_tieu_chi!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
@@ -981,4 +1003,71 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>